<commit_message>
Add more test cases
</commit_message>
<xml_diff>
--- a/docs/Lunar_TestCases.xlsx
+++ b/docs/Lunar_TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Калина Нончева\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Калина Нончева\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A682D76-5815-4D0A-BD18-6EF92BE18030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A0B439-F8BB-4464-922B-F3A04B036417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A318E8DC-3BAF-461E-927A-906EB1266462}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A318E8DC-3BAF-461E-927A-906EB1266462}"/>
   </bookViews>
   <sheets>
     <sheet name="BackEnd.cpp" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="43">
   <si>
     <t>Details</t>
   </si>
@@ -106,9 +106,6 @@
     <t>08.02.2022 17:25</t>
   </si>
   <si>
-    <t>08.02.2022 17:30</t>
-  </si>
-  <si>
     <t>Test_02</t>
   </si>
   <si>
@@ -127,7 +124,46 @@
     <t>To display the table</t>
   </si>
   <si>
-    <t>08.02.2022 17:40</t>
+    <t>Test_03</t>
+  </si>
+  <si>
+    <t>Entering data</t>
+  </si>
+  <si>
+    <t>To start the application</t>
+  </si>
+  <si>
+    <t>08.02.2022 18:15</t>
+  </si>
+  <si>
+    <t>08.02.2022 18:19</t>
+  </si>
+  <si>
+    <t>08.02.2022 18:20</t>
+  </si>
+  <si>
+    <t>void innitDataBase()</t>
+  </si>
+  <si>
+    <t>Prints the table</t>
+  </si>
+  <si>
+    <t>08.02.2022 18:26</t>
+  </si>
+  <si>
+    <t>08.02.2022 18:27</t>
+  </si>
+  <si>
+    <t>Test_04</t>
+  </si>
+  <si>
+    <t>void getInput()</t>
+  </si>
+  <si>
+    <t>Prints the data</t>
+  </si>
+  <si>
+    <t>08.02.2022 18:33</t>
   </si>
 </sst>
 </file>
@@ -184,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -292,34 +328,29 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,31 +360,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -363,73 +381,98 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
+  <dxfs count="44">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -440,55 +483,81 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -548,24 +617,595 @@
           <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
         <bottom/>
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -573,92 +1213,11 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+        <top/>
         <bottom/>
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -667,34 +1226,34 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -722,30 +1281,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9F71E2B-DA9D-4B54-B8CF-56700481CF89}" name="Table61236" displayName="Table61236" ref="B9:G10" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
-  <autoFilter ref="B9:G10" xr:uid="{B9F71E2B-DA9D-4B54-B8CF-56700481CF89}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9F71E2B-DA9D-4B54-B8CF-56700481CF89}" name="Table61236" displayName="Table61236" ref="B9:G11" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40" totalsRowBorderDxfId="39">
+  <autoFilter ref="B9:G11" xr:uid="{B9F71E2B-DA9D-4B54-B8CF-56700481CF89}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BD57BFEE-7983-4540-BF08-43D68694351D}" name="Number step" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{9725D7AE-CE45-4E44-B51C-18555BDAA650}" name="Description" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{C5E64368-8DC2-4CEC-8CFB-CEA2C550C4AB}" name="Test Data" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{E3563205-2093-4C29-B589-AEBFF4499DBD}" name="Expectations" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{64061350-3BB4-433A-9388-94A0D456A241}" name="Actual Result" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{BC3CD63A-5C6B-4286-9F5E-9038D9F6ECDA}" name="Status" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{BD57BFEE-7983-4540-BF08-43D68694351D}" name="Number step" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{9725D7AE-CE45-4E44-B51C-18555BDAA650}" name="Description" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{C5E64368-8DC2-4CEC-8CFB-CEA2C550C4AB}" name="Test Data" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{E3563205-2093-4C29-B589-AEBFF4499DBD}" name="Expectations" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{64061350-3BB4-433A-9388-94A0D456A241}" name="Actual Result" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{BC3CD63A-5C6B-4286-9F5E-9038D9F6ECDA}" name="Status" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6F87464-5784-4F49-81E1-BF7B456FC07E}" name="Table612363" displayName="Table612363" ref="B21:G22" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
-  <autoFilter ref="B21:G22" xr:uid="{D6F87464-5784-4F49-81E1-BF7B456FC07E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6F87464-5784-4F49-81E1-BF7B456FC07E}" name="Table612363" displayName="Table612363" ref="B21:G23" totalsRowShown="0" headerRowDxfId="38" dataDxfId="24" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+  <autoFilter ref="B21:G23" xr:uid="{D6F87464-5784-4F49-81E1-BF7B456FC07E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{24DE775F-8DA4-45D2-BBEF-D6D3F224111B}" name="Number step" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B94882E8-FD71-4F17-8E34-C558E4C86B40}" name="Description" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{29C4BA4F-0DF0-4602-B471-0406C4989A78}" name="Test Data" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{2C15706E-BAC2-41A3-9229-FCDF2BF0801D}" name="Expectations" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{69620B87-58D0-47E2-B934-CB83F1952D9E}" name="Actual Result" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{23662DE0-FFA1-48FD-81A4-1E5EABE272E7}" name="Status" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{24DE775F-8DA4-45D2-BBEF-D6D3F224111B}" name="Number step" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{B94882E8-FD71-4F17-8E34-C558E4C86B40}" name="Description" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{29C4BA4F-0DF0-4602-B471-0406C4989A78}" name="Test Data" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{2C15706E-BAC2-41A3-9229-FCDF2BF0801D}" name="Expectations" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{69620B87-58D0-47E2-B934-CB83F1952D9E}" name="Actual Result" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{23662DE0-FFA1-48FD-81A4-1E5EABE272E7}" name="Status" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{27D12283-894D-4D26-A211-E0B8838CD628}" name="Table612364" displayName="Table612364" ref="B9:G10" totalsRowShown="0" headerRowDxfId="34" dataDxfId="17" headerRowBorderDxfId="32" tableBorderDxfId="33" totalsRowBorderDxfId="31">
+  <autoFilter ref="B9:G10" xr:uid="{27D12283-894D-4D26-A211-E0B8838CD628}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{3DB24851-BB6B-464F-A32F-BC92B2F894D7}" name="Number step" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{43178B2C-34E5-4FD0-80D4-EBCDD2571296}" name="Description" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{A69FAC80-028C-4625-AF8F-396D21CF8822}" name="Test Data" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{C0EFBA6B-5795-4C03-8F1E-3B3C4449EA83}" name="Expectations" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{9F48AF64-9EC9-4228-9947-A83BF5ABBEFF}" name="Actual Result" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{E003AABE-EA3F-4D09-AA73-E01B99659797}" name="Status" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8958A56D-A901-447B-891C-ABE52675C5ED}" name="Table6123645" displayName="Table6123645" ref="B20:G21" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="B20:G21" xr:uid="{8958A56D-A901-447B-891C-ABE52675C5ED}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{7610045E-A0EF-48A5-86D1-C57525AF259C}" name="Number step" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{2514890D-7A95-4269-AE53-2C0177E90674}" name="Description" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{1F79A521-910E-4F2E-904F-09DEF3D8DA7E}" name="Test Data" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{BBE97B07-9EDD-4671-BB13-C07C230D37FF}" name="Expectations" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{0556EDEC-FE49-4454-B2D2-F548235A7CFD}" name="Actual Result" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{92C69008-99E4-4E97-B533-3869B55B0725}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1048,10 +1637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EAFFD2-E5C7-4345-962D-A94815B4D10B}">
-  <dimension ref="B2:G22"/>
+  <dimension ref="B2:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,63 +1654,63 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="21" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>23</v>
+      <c r="E6" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -1135,103 +1724,121 @@
       <c r="G8" s="19"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="13">
+      <c r="B10" s="20">
         <v>1</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="21"/>
+      <c r="E10" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="6">
+        <v>2</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="D17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="21" t="s">
+      <c r="B18" s="14"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>30</v>
+      <c r="E18" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
@@ -1245,53 +1852,73 @@
       <c r="G20" s="19"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="13">
+      <c r="B22" s="20">
         <v>1</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="21"/>
+      <c r="E22" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="6">
+        <v>2</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="21">
         <v>10</v>
       </c>
-      <c r="E22" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="14" t="s">
+      <c r="E23" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G23" s="20" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="B20:G20"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -1303,14 +1930,261 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90314F01-8834-412D-B03D-FB1C47125FBB}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="14"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="14"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="19"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>